<commit_message>
añadidos ejercicios excel 4 de noviembre
</commit_message>
<xml_diff>
--- a/m1/unidad3/Practicas/20191030/Codigos de moda.xlsx
+++ b/m1/unidad3/Practicas/20191030/Codigos de moda.xlsx
@@ -505,7 +505,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +539,10 @@
         <f>MID(A2,FIND("-",A2,1)+1,2)</f>
         <v>65</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4" t="str">
+        <f>MID(A2,FIND("-",A2,1)+3,3)</f>
+        <v>XL</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -553,7 +556,10 @@
         <f t="shared" ref="C3:C8" si="1">MID(A3,FIND("-",A3,1)+1,2)</f>
         <v>65</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="str">
+        <f t="shared" ref="D3:D8" si="2">MID(A3,FIND("-",A3,1)+3,3)</f>
+        <v>XXL</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -567,7 +573,10 @@
         <f t="shared" si="1"/>
         <v>06</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>M</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -581,7 +590,10 @@
         <f t="shared" si="1"/>
         <v>06</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>L</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -595,7 +607,10 @@
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>XL</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -609,7 +624,10 @@
         <f t="shared" si="1"/>
         <v>07</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>XXS</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -623,7 +641,10 @@
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>XS</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>